<commit_message>
Moster Table element 추가, hud object 추가
</commit_message>
<xml_diff>
--- a/Project_C/Assets/ExcelTable/MonsterTable.xlsx
+++ b/Project_C/Assets/ExcelTable/MonsterTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOW2_400_203\Desktop\TeamIdentity\Project_C\Assets\ExcelTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Park\Desktop\Park\Project_C\Project_C\Assets\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0920E2-4AE3-4F89-B113-F5AE60A74374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="645" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterTable" sheetId="1" r:id="rId1"/>
@@ -19,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
   <si>
     <t>i_Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -262,10 +255,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>E_Stun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이 몬스터는 공격에 성공할 시 적에게 _만큼 슬로우를 부여하고 체력이 _이하로 줄어들게 되면 자신을 기준으로 한 원형의 범위 힐을 초당 _만큼 준다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -315,13 +304,33 @@
   </si>
   <si>
     <t>이 몬스터는 공격을 받고 죽지 않으면 고블린 취객을 _마리 소환합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_EffectOffset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_HUDOffset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이펙트 y 오프셋(픽셀)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hud y 오프셋(픽셀)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E_GiveStun</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -968,21 +977,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="164.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="164.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,24 +1016,30 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="7" t="s">
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1045,40 +1062,46 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>74</v>
-      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>501</v>
       </c>
@@ -1100,18 +1123,18 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="1">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L3" s="1" t="s">
         <v>32</v>
       </c>
@@ -1121,20 +1144,26 @@
       <c r="N3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="1">
         <v>2</v>
       </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
       <c r="R3" s="1">
         <v>0</v>
       </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>502</v>
       </c>
@@ -1156,15 +1185,15 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="1">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1">
+        <v>100</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
@@ -1177,11 +1206,11 @@
       <c r="N4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
+      <c r="O4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="Q4" s="1">
         <v>0</v>
@@ -1189,8 +1218,14 @@
       <c r="R4" s="1">
         <v>0</v>
       </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>503</v>
       </c>
@@ -1212,18 +1247,18 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="1">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1">
+        <v>30</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1233,20 +1268,26 @@
       <c r="N5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="1">
         <v>1.5</v>
       </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
       <c r="R5" s="1">
         <v>0</v>
       </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>504</v>
       </c>
@@ -1268,41 +1309,47 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="1">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="M6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="1">
         <v>1</v>
       </c>
-      <c r="P6" s="1">
+      <c r="R6" s="1">
         <v>2</v>
       </c>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>505</v>
       </c>
@@ -1324,18 +1371,18 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="1">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1345,20 +1392,26 @@
       <c r="N7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="1">
         <v>1</v>
       </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
       <c r="R7" s="1">
         <v>0</v>
       </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>506</v>
       </c>
@@ -1380,41 +1433,47 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="1">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>61</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="N8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="1">
         <v>1</v>
       </c>
-      <c r="P8" s="1">
+      <c r="R8" s="1">
         <v>5</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="S8" s="1">
         <v>0.2</v>
       </c>
-      <c r="R8" s="1">
+      <c r="T8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>507</v>
       </c>
@@ -1436,18 +1495,18 @@
       <c r="G9" s="1">
         <v>100</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="1">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1">
+        <v>30</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1457,11 +1516,11 @@
       <c r="N9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="1">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0</v>
+      <c r="O9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="Q9" s="1">
         <v>0</v>
@@ -1469,8 +1528,14 @@
       <c r="R9" s="1">
         <v>0</v>
       </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>508</v>
       </c>
@@ -1492,41 +1557,47 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="1">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J10" t="s">
-        <v>65</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="N10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="1">
         <v>2</v>
       </c>
-      <c r="P10" s="1">
+      <c r="R10" s="1">
         <v>2</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="S10" s="1">
         <v>512</v>
       </c>
-      <c r="R10" s="3">
+      <c r="T10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>509</v>
       </c>
@@ -1548,41 +1619,47 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="H11" s="1">
+        <v>15</v>
+      </c>
+      <c r="I11" s="1">
+        <v>30</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="M11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="1">
         <v>0.25</v>
       </c>
-      <c r="P11" s="1">
+      <c r="R11" s="1">
         <v>100</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="S11" s="1">
         <v>15</v>
       </c>
-      <c r="R11" s="1">
+      <c r="T11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>510</v>
       </c>
@@ -1604,18 +1681,18 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="H12" s="1">
+        <v>15</v>
+      </c>
+      <c r="I12" s="1">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1625,28 +1702,34 @@
       <c r="N12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="1">
         <v>507</v>
       </c>
-      <c r="P12" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>0</v>
-      </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>511</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D13" s="1">
         <v>5</v>
@@ -1660,14 +1743,14 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>32</v>
+      <c r="H13" s="1">
+        <v>15</v>
+      </c>
+      <c r="I13" s="1">
+        <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>32</v>
@@ -1681,11 +1764,11 @@
       <c r="N13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
+      <c r="O13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="Q13" s="1">
         <v>0</v>
@@ -1693,16 +1776,22 @@
       <c r="R13" s="1">
         <v>0</v>
       </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>512</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -1716,18 +1805,18 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="H14" s="1">
+        <v>15</v>
+      </c>
+      <c r="I14" s="1">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1737,11 +1826,11 @@
       <c r="N14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="1">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0</v>
+      <c r="O14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="Q14" s="1">
         <v>0</v>
@@ -1749,16 +1838,22 @@
       <c r="R14" s="1">
         <v>0</v>
       </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>513</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -1772,18 +1867,18 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="H15" s="1">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1">
+        <v>30</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1793,136 +1888,82 @@
       <c r="N15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" s="1">
         <v>1</v>
       </c>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0</v>
-      </c>
       <c r="R15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="S15" s="1">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="K1:P1"/>
+    <mergeCell ref="Q1:T1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:I1 A2:N2">
+  <conditionalFormatting sqref="A1:K1 A2:P2">
     <cfRule type="expression" dxfId="10" priority="13">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1">
+  <conditionalFormatting sqref="Q1">
     <cfRule type="expression" dxfId="9" priority="12">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:P2">
+  <conditionalFormatting sqref="Q2:R2">
     <cfRule type="expression" dxfId="8" priority="11">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:H4 A5:I8 A9:H9 A11:H11">
+  <conditionalFormatting sqref="A3:J3 A11:G11 J11 J9 J5:K8 A4:G9 J4 H4:I15">
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>$A3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:H10">
+  <conditionalFormatting sqref="A10:G10 J10">
     <cfRule type="expression" dxfId="6" priority="8">
       <formula>$A10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:H10">
+  <conditionalFormatting sqref="B10:G10 J10">
     <cfRule type="expression" dxfId="5" priority="7">
       <formula>$A10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:H9">
+  <conditionalFormatting sqref="B9:G9 J9">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>$A9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+  <conditionalFormatting sqref="J14">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$A14&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
+  <conditionalFormatting sqref="J14">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>$A14&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O12">
+  <conditionalFormatting sqref="Q12">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>$A12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:R2">
+  <conditionalFormatting sqref="S2:T2">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>

</xml_diff>

<commit_message>
hud raycast off, attack particle angle calc
</commit_message>
<xml_diff>
--- a/Project_C/Assets/ExcelTable/MonsterTable.xlsx
+++ b/Project_C/Assets/ExcelTable/MonsterTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOW2_400_204\Desktop\TeamIdentity\Project_C\Assets\ExcelTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Main\TeamIdentity\Project_C\Assets\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BE0D35-2047-46B7-9C92-AD3C20625860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="27990" windowHeight="14760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterTable" sheetId="1" r:id="rId1"/>
@@ -314,22 +315,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hud y 오프셋(픽셀)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E_GiveStun</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>이펙트 y 좌표(1=&gt;iso tile height)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hud y 좌표(1=&gt;iso tile height)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -976,11 +977,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -988,7 +989,7 @@
     <col min="2" max="2" width="14.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="31.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="164.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1061,10 +1062,10 @@
         <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>16</v>
@@ -1123,10 +1124,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>15</v>
+        <v>0.2</v>
       </c>
       <c r="I3" s="1">
-        <v>100</v>
+        <v>0.8</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>30</v>
@@ -1185,10 +1186,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="I4" s="1">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>35</v>
@@ -1247,10 +1248,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <v>15</v>
+        <v>0.4</v>
       </c>
       <c r="I5" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>38</v>
@@ -1309,10 +1310,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>15</v>
+        <v>0.4</v>
       </c>
       <c r="I6" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>57</v>
@@ -1371,10 +1372,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>15</v>
+        <v>0.4</v>
       </c>
       <c r="I7" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>44</v>
@@ -1433,10 +1434,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>15</v>
+        <v>0.2</v>
       </c>
       <c r="I8" s="1">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>60</v>
@@ -1495,10 +1496,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>15</v>
+        <v>0.5</v>
       </c>
       <c r="I9" s="1">
-        <v>100</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>48</v>
@@ -1557,10 +1558,10 @@
         <v>100</v>
       </c>
       <c r="H10" s="1">
-        <v>15</v>
+        <v>0.2</v>
       </c>
       <c r="I10" s="1">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>64</v>
@@ -1569,7 +1570,7 @@
         <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>31</v>
@@ -1619,10 +1620,10 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <v>15</v>
+        <v>0.2</v>
       </c>
       <c r="I11" s="1">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>65</v>
@@ -1681,10 +1682,10 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>15</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="1">
-        <v>100</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>66</v>
@@ -1743,10 +1744,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>15</v>
+        <v>0.2</v>
       </c>
       <c r="I13" s="1">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>69</v>
@@ -1805,10 +1806,10 @@
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>15</v>
+        <v>0.2</v>
       </c>
       <c r="I14" s="1">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>74</v>
@@ -1867,10 +1868,10 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <v>15</v>
+        <v>0.2</v>
       </c>
       <c r="I15" s="1">
-        <v>100</v>
+        <v>0.9</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>77</v>
@@ -1928,42 +1929,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:J3 A11:G11 J11 J9 J5:K8 A4:G9 J4 H4:I15">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>$A3&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:G10 J10">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$A10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:G10 J10">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$A10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:G9 J9">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$A9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$A14&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$A14&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>